<commit_message>
move files outside of html folder
</commit_message>
<xml_diff>
--- a/conditions.xlsx
+++ b/conditions.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AA040D-4F5D-4057-8D63-826CCB834A10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBCE670-69FC-4FAF-9C0F-53EEB414C21E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,34 +124,34 @@
     <t>Sound_N</t>
   </si>
   <si>
+    <t>Beep</t>
+  </si>
+  <si>
+    <t>KeyNum</t>
+  </si>
+  <si>
+    <t>Symb</t>
+  </si>
+  <si>
+    <t>Symb_R</t>
+  </si>
+  <si>
+    <t>Symb_G</t>
+  </si>
+  <si>
+    <t>StimNum</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>media/coin.wav</t>
+  </si>
+  <si>
     <t>media/buzz.wav</t>
   </si>
   <si>
-    <t>media/coin.wav</t>
-  </si>
-  <si>
-    <t>Beep</t>
-  </si>
-  <si>
     <t>media/beep.wav</t>
-  </si>
-  <si>
-    <t>KeyNum</t>
-  </si>
-  <si>
-    <t>Symb</t>
-  </si>
-  <si>
-    <t>Symb_R</t>
-  </si>
-  <si>
-    <t>Symb_G</t>
-  </si>
-  <si>
-    <t>StimNum</t>
-  </si>
-  <si>
-    <t>Key</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -488,22 +488,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
       </c>
       <c r="G1" t="s">
         <v>30</v>
@@ -521,7 +521,7 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -553,13 +553,13 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>